<commit_message>
edit device query setting
</commit_message>
<xml_diff>
--- a/uploads/import_sim_ids.xlsx
+++ b/uploads/import_sim_ids.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usman\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hamza Dawood\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CADF02C-335C-4933-9FA6-1B13B54A2C03}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2462537E-34E2-46DF-B8B1-4C47DC29BEFF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{8AD02A7E-7BF6-40BB-AAC7-5F214A7BCE78}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8AD02A7E-7BF6-40BB-AAC7-5F214A7BCE78}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="5">
   <si>
     <t>sim_id</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>expiry_date</t>
+  </si>
+  <si>
+    <t>26-3-2019</t>
+  </si>
+  <si>
+    <t>26-4-2019</t>
   </si>
 </sst>
 </file>
@@ -388,7 +394,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -408,19 +414,43 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -428,40 +458,88 @@
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>